<commit_message>
Removing Isolation code and updating files
</commit_message>
<xml_diff>
--- a/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI\PowerBI-visuals\documents\Published\DataInsights\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>S no</t>
   </si>
@@ -189,37 +189,15 @@
     <t>Similar for Min, average and constant line</t>
   </si>
   <si>
-    <t>Isolation</t>
-  </si>
-  <si>
     <t>1.Select bar/ Column chart from view as
 2. Go to format pane
 3. Analytics &gt; Toggle on Max Line</t>
   </si>
   <si>
-    <t>1.Select bar/column/ brick chart
-2. click Drag the mouse to select the bars/brick
-3. click on isolate</t>
-  </si>
-  <si>
-    <t>A blue box is drawn on dragging.
-On leaving the mouse the opacity of bars not selected is reduced
-Only the selected bars/bricks are rendered</t>
-  </si>
-  <si>
-    <t>Verify Isolation functionality(Not available for table)</t>
-  </si>
-  <si>
     <t>Reset</t>
   </si>
   <si>
     <t>Verify reset(Reset works only for isolation)</t>
-  </si>
-  <si>
-    <t>Perform isolation as in 9</t>
-  </si>
-  <si>
-    <t>Click reset. The visual displays all the data</t>
   </si>
   <si>
     <t>Undo</t>
@@ -351,6 +329,14 @@
   </si>
   <si>
     <t>Top menu bar disappear. Axis labels are present which allows you to change the axis values</t>
+  </si>
+  <si>
+    <t>1. Click on any bar/column/brick
+2. Click on Reset button</t>
+  </si>
+  <si>
+    <t>The selected bar/brick/column gets higher opacity and others get lower opacity
+Chart is redrawn and opacity gets reset to normal</t>
   </si>
 </sst>
 </file>
@@ -721,7 +707,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +715,7 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="5" max="5" width="67.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -902,10 +888,10 @@
         <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -921,80 +907,68 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1022,13 +996,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1036,10 +1010,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1047,10 +1021,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1058,10 +1032,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1069,10 +1043,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1080,10 +1054,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1091,10 +1065,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1102,10 +1076,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,10 +1087,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,10 +1098,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,10 +1109,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1146,10 +1120,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,7 +1131,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1165,10 +1139,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1176,10 +1150,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1187,7 +1161,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,20 +1169,20 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1216,10 +1190,10 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1227,25 +1201,25 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,10 +1227,10 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,10 +1238,10 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>